<commit_message>
feature/up-download: making delete file
</commit_message>
<xml_diff>
--- a/uploads/Meeting_22.08.04.xlsx
+++ b/uploads/Meeting_22.08.04.xlsx
@@ -287,7 +287,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" mc:Ignorable="x14ac">
   <numFmts count="0"/>
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -298,12 +298,6 @@
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
     </font>
@@ -377,7 +371,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="12">
     <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0"/>
     <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
       <alignment horizontal="general"/>
@@ -406,13 +400,10 @@
     <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="2" applyFont="1" fillId="0" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="0" fontId="0" fillId="0" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="3" applyFont="1" fillId="0" applyAlignment="1">
+    <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="2" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
   </cellXfs>
@@ -723,7 +714,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" style="11" width="3.1478571428571427" customWidth="1" bestFit="1"/>
+    <col min="1" max="1" style="10" width="3.1478571428571427" customWidth="1" bestFit="1"/>
     <col min="2" max="2" style="4" width="13.576428571428572" customWidth="1" bestFit="1"/>
     <col min="3" max="3" style="4" width="78.57642857142856" customWidth="1" bestFit="1"/>
     <col min="4" max="4" style="3" width="22.005" customWidth="1" bestFit="1"/>
@@ -732,8 +723,8 @@
   <sheetData>
     <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="18.75">
       <c r="A1" s="9"/>
-      <c r="B1" s="10"/>
-      <c r="C1" s="10"/>
+      <c r="B1" s="2"/>
+      <c r="C1" s="2"/>
       <c r="D1" s="1"/>
       <c r="E1" s="1"/>
     </row>
@@ -741,16 +732,16 @@
       <c r="A2" s="9">
         <v>1</v>
       </c>
-      <c r="B2" s="12" t="s">
+      <c r="B2" s="11" t="s">
         <v>25</v>
       </c>
-      <c r="C2" s="10"/>
+      <c r="C2" s="2"/>
       <c r="D2" s="1"/>
       <c r="E2" s="1"/>
     </row>
     <row x14ac:dyDescent="0.25" r="3" customHeight="1" ht="18.75">
       <c r="A3" s="9"/>
-      <c r="B3" s="10"/>
+      <c r="B3" s="2"/>
       <c r="C3" s="2" t="s">
         <v>26</v>
       </c>
@@ -761,7 +752,7 @@
     </row>
     <row x14ac:dyDescent="0.25" r="4" customHeight="1" ht="18.75">
       <c r="A4" s="9"/>
-      <c r="B4" s="10"/>
+      <c r="B4" s="2"/>
       <c r="C4" s="2" t="s">
         <v>28</v>
       </c>
@@ -772,7 +763,7 @@
     </row>
     <row x14ac:dyDescent="0.25" r="5" customHeight="1" ht="18.75">
       <c r="A5" s="9"/>
-      <c r="B5" s="10"/>
+      <c r="B5" s="2"/>
       <c r="C5" s="2" t="s">
         <v>30</v>
       </c>
@@ -785,7 +776,7 @@
     </row>
     <row x14ac:dyDescent="0.25" r="6" customHeight="1" ht="18.75">
       <c r="A6" s="9"/>
-      <c r="B6" s="10"/>
+      <c r="B6" s="2"/>
       <c r="C6" s="2" t="s">
         <v>33</v>
       </c>
@@ -798,7 +789,7 @@
     </row>
     <row x14ac:dyDescent="0.25" r="7" customHeight="1" ht="18.75">
       <c r="A7" s="9"/>
-      <c r="B7" s="10"/>
+      <c r="B7" s="2"/>
       <c r="C7" s="2" t="s">
         <v>36</v>
       </c>
@@ -807,7 +798,7 @@
     </row>
     <row x14ac:dyDescent="0.25" r="8" customHeight="1" ht="18.75">
       <c r="A8" s="9"/>
-      <c r="B8" s="10"/>
+      <c r="B8" s="2"/>
       <c r="C8" s="2" t="s">
         <v>37</v>
       </c>
@@ -816,7 +807,7 @@
     </row>
     <row x14ac:dyDescent="0.25" r="9" customHeight="1" ht="18.75">
       <c r="A9" s="9"/>
-      <c r="B9" s="10"/>
+      <c r="B9" s="2"/>
       <c r="C9" s="2" t="s">
         <v>38</v>
       </c>
@@ -827,7 +818,7 @@
     </row>
     <row x14ac:dyDescent="0.25" r="10" customHeight="1" ht="18.75">
       <c r="A10" s="9"/>
-      <c r="B10" s="10"/>
+      <c r="B10" s="2"/>
       <c r="C10" s="2" t="s">
         <v>40</v>
       </c>
@@ -838,7 +829,7 @@
     </row>
     <row x14ac:dyDescent="0.25" r="11" customHeight="1" ht="18.75">
       <c r="A11" s="9"/>
-      <c r="B11" s="10"/>
+      <c r="B11" s="2"/>
       <c r="C11" s="2" t="s">
         <v>42</v>
       </c>
@@ -849,31 +840,31 @@
     </row>
     <row x14ac:dyDescent="0.25" r="12" customHeight="1" ht="18.75">
       <c r="A12" s="9"/>
-      <c r="B12" s="10"/>
-      <c r="C12" s="10"/>
+      <c r="B12" s="2"/>
+      <c r="C12" s="2"/>
       <c r="D12" s="1"/>
       <c r="E12" s="1"/>
     </row>
     <row x14ac:dyDescent="0.25" r="13" customHeight="1" ht="18.75">
       <c r="A13" s="9"/>
-      <c r="B13" s="10"/>
-      <c r="C13" s="10"/>
+      <c r="B13" s="2"/>
+      <c r="C13" s="2"/>
       <c r="D13" s="1"/>
       <c r="E13" s="1"/>
     </row>
     <row x14ac:dyDescent="0.25" r="14" customHeight="1" ht="18.75">
       <c r="A14" s="9"/>
-      <c r="B14" s="10"/>
-      <c r="C14" s="10"/>
+      <c r="B14" s="2"/>
+      <c r="C14" s="2"/>
       <c r="D14" s="1"/>
       <c r="E14" s="1"/>
     </row>
     <row x14ac:dyDescent="0.25" r="15" customHeight="1" ht="18.75">
       <c r="A15" s="9"/>
-      <c r="B15" s="12" t="s">
+      <c r="B15" s="11" t="s">
         <v>44</v>
       </c>
-      <c r="C15" s="10"/>
+      <c r="C15" s="2"/>
       <c r="D15" s="1"/>
       <c r="E15" s="1"/>
     </row>
@@ -882,7 +873,7 @@
       <c r="B16" s="2" t="s">
         <v>45</v>
       </c>
-      <c r="C16" s="10"/>
+      <c r="C16" s="2"/>
       <c r="D16" s="2" t="s">
         <v>46</v>
       </c>
@@ -893,7 +884,7 @@
       <c r="B17" s="2" t="s">
         <v>47</v>
       </c>
-      <c r="C17" s="10"/>
+      <c r="C17" s="2"/>
       <c r="D17" s="1"/>
       <c r="E17" s="1"/>
     </row>
@@ -912,31 +903,31 @@
     </row>
     <row x14ac:dyDescent="0.25" r="19" customHeight="1" ht="18.75">
       <c r="A19" s="9"/>
-      <c r="B19" s="10"/>
-      <c r="C19" s="10"/>
+      <c r="B19" s="2"/>
+      <c r="C19" s="2"/>
       <c r="D19" s="1"/>
       <c r="E19" s="1"/>
     </row>
     <row x14ac:dyDescent="0.25" r="20" customHeight="1" ht="18.75">
       <c r="A20" s="9"/>
-      <c r="B20" s="10"/>
-      <c r="C20" s="10"/>
+      <c r="B20" s="2"/>
+      <c r="C20" s="2"/>
       <c r="D20" s="1"/>
       <c r="E20" s="1"/>
     </row>
     <row x14ac:dyDescent="0.25" r="21" customHeight="1" ht="18.75">
       <c r="A21" s="9"/>
-      <c r="B21" s="10"/>
-      <c r="C21" s="10"/>
+      <c r="B21" s="2"/>
+      <c r="C21" s="2"/>
       <c r="D21" s="1"/>
       <c r="E21" s="1"/>
     </row>
     <row x14ac:dyDescent="0.25" r="22" customHeight="1" ht="18.75">
       <c r="A22" s="9"/>
-      <c r="B22" s="12" t="s">
+      <c r="B22" s="11" t="s">
         <v>14</v>
       </c>
-      <c r="C22" s="10"/>
+      <c r="C22" s="2"/>
       <c r="D22" s="1"/>
       <c r="E22" s="1"/>
     </row>
@@ -945,30 +936,30 @@
       <c r="B23" s="2" t="s">
         <v>51</v>
       </c>
-      <c r="C23" s="10"/>
+      <c r="C23" s="2"/>
       <c r="D23" s="1"/>
       <c r="E23" s="1"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="24" customHeight="1" ht="17.25">
+    <row x14ac:dyDescent="0.25" r="24" customHeight="1" ht="18.75">
       <c r="A24" s="9"/>
-      <c r="B24" s="10"/>
-      <c r="C24" s="10"/>
+      <c r="B24" s="2"/>
+      <c r="C24" s="2"/>
       <c r="D24" s="1"/>
       <c r="E24" s="1"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="25" customHeight="1" ht="17.25">
+    <row x14ac:dyDescent="0.25" r="25" customHeight="1" ht="18.75">
       <c r="A25" s="9"/>
-      <c r="B25" s="10"/>
-      <c r="C25" s="10"/>
+      <c r="B25" s="2"/>
+      <c r="C25" s="2"/>
       <c r="D25" s="1"/>
       <c r="E25" s="1"/>
     </row>
     <row x14ac:dyDescent="0.25" r="26" customHeight="1" ht="18.75">
       <c r="A26" s="9"/>
-      <c r="B26" s="12" t="s">
+      <c r="B26" s="11" t="s">
         <v>52</v>
       </c>
-      <c r="C26" s="10"/>
+      <c r="C26" s="2"/>
       <c r="D26" s="1"/>
       <c r="E26" s="1"/>
     </row>
@@ -999,7 +990,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" style="11" width="4.433571428571429" customWidth="1" bestFit="1"/>
+    <col min="1" max="1" style="10" width="4.433571428571429" customWidth="1" bestFit="1"/>
     <col min="2" max="2" style="4" width="63.005" customWidth="1" bestFit="1"/>
     <col min="3" max="3" style="3" width="12.43357142857143" customWidth="1" bestFit="1"/>
     <col min="4" max="4" style="3" width="46.86214285714286" customWidth="1" bestFit="1"/>
@@ -1117,13 +1108,13 @@
     </row>
     <row x14ac:dyDescent="0.25" r="13" customHeight="1" ht="17.25">
       <c r="A13" s="9"/>
-      <c r="B13" s="10"/>
+      <c r="B13" s="2"/>
       <c r="C13" s="1"/>
       <c r="D13" s="1"/>
     </row>
     <row x14ac:dyDescent="0.25" r="14" customHeight="1" ht="17.25">
       <c r="A14" s="9"/>
-      <c r="B14" s="10"/>
+      <c r="B14" s="2"/>
       <c r="C14" s="1"/>
       <c r="D14" s="1"/>
     </row>

</xml_diff>